<commit_message>
Update Копия CAM_DVB-CI_rev.1.1_release BOM-offer(1).xlsx
</commit_message>
<xml_diff>
--- a/CAM-ALTERA_STM/Производство/Копия CAM_DVB-CI_rev.1.1_release BOM-offer(1).xlsx
+++ b/CAM-ALTERA_STM/Производство/Копия CAM_DVB-CI_rev.1.1_release BOM-offer(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\CASS\CAM-ALTERA_STM\Производство\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9360B039-CEAB-4CA7-B909-A8C09BCF7F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{271DD60B-1C06-4EEE-8C0C-8E784E9FB1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="246">
   <si>
     <t>Designator</t>
   </si>
@@ -59,10 +59,10 @@
     <t>HelpURL</t>
   </si>
   <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>Client Response</t>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>REPLY</t>
   </si>
   <si>
     <t>P/N</t>
@@ -412,6 +412,12 @@
     <t>discontinued</t>
   </si>
   <si>
+    <t>Позицию IC7 W25Q64CVSSIG, можно заменить на W25Q64JVSSIQ.</t>
+  </si>
+  <si>
+    <t>W25Q64JVSSIQ</t>
+  </si>
+  <si>
     <t>WINBIND</t>
   </si>
   <si>
@@ -424,9 +430,18 @@
     <t>Connector Card Bus Socket</t>
   </si>
   <si>
+    <t xml:space="preserve">1. Позиция J1 - IC9-68RD-0.635SF – альтернативный вариант PCFSMT-K1-RLE10-B059C-GW другой завод устанавливает такие разъёмы. Как альтернатива еще есть разъемы: IC1FA-68PD-1.27DS(72), IC1F-68RD-1.27SF(52), IC1K-68RD-1.27SF(71), 10014744-002SLF, 5146228-4, IC1HA-68RD-1.27SH(51), IC1BB-68RD-1.27SH, 5146233-1. </t>
+  </si>
+  <si>
+    <t>IC1F-68RD-1.27SF</t>
+  </si>
+  <si>
     <t>HIROSE</t>
   </si>
   <si>
+    <t>22-24weeks</t>
+  </si>
+  <si>
     <t>J2</t>
   </si>
   <si>
@@ -436,6 +451,9 @@
     <t>Connector, Header, Pitch 2mm, H=4.3mm</t>
   </si>
   <si>
+    <t>Позиции J2-J3 не закупаем и не монтируем.</t>
+  </si>
+  <si>
     <t>DS1026-01-1x6S8BV</t>
   </si>
   <si>
@@ -454,10 +472,19 @@
     <t>Please confirm the alternative model number.</t>
   </si>
   <si>
+    <t xml:space="preserve"> Позиции J2-J3 не закупаем и не монтируем.</t>
+  </si>
+  <si>
     <t>2005FV-2x5P</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>HanElectricity(</t>
     </r>
     <r>
@@ -694,6 +721,12 @@
   </si>
   <si>
     <t>Few available, alternatives recommended</t>
+  </si>
+  <si>
+    <t>Позиция U1 EP4CE22E22C6N в каком количестве есть? Плюс возможно ставить варианты с любым индексом в конце EP4CE22E22C6N (I7N, C8N) так же можно установить вариант с меньшим количеством ячеек EP4CE15E22I7N нас устроит любой индекс в конце микросхемы!</t>
+  </si>
+  <si>
+    <t>EP4CE15E22I7N</t>
   </si>
   <si>
     <t>Intel</t>
@@ -978,7 +1011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1030,9 +1063,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1043,6 +1077,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1403,21 +1440,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X25" workbookViewId="0">
-      <selection activeCell="AG38" sqref="AG38"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="9.77734375" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" customWidth="1"/>
     <col min="8" max="8" width="9.109375" customWidth="1"/>
-    <col min="9" max="9" width="50.109375" customWidth="1"/>
+    <col min="9" max="9" width="33.77734375" customWidth="1"/>
     <col min="10" max="10" width="15.109375" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
     <col min="12" max="12" width="9.33203125" customWidth="1"/>
@@ -1495,17 +1532,17 @@
       <c r="Q1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="S1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="35" t="s">
         <v>18</v>
       </c>
       <c r="U1" s="6"/>
-      <c r="V1" s="34" t="s">
+      <c r="V1" s="36" t="s">
         <v>13</v>
       </c>
       <c r="W1" s="17" t="s">
@@ -1514,17 +1551,17 @@
       <c r="X1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="31" t="s">
+      <c r="Y1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="32" t="s">
+      <c r="Z1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="33" t="s">
+      <c r="AA1" s="35" t="s">
         <v>18</v>
       </c>
       <c r="AB1" s="6"/>
-      <c r="AC1" s="34" t="s">
+      <c r="AC1" s="36" t="s">
         <v>13</v>
       </c>
       <c r="AD1" s="17" t="s">
@@ -1533,10 +1570,10 @@
       <c r="AE1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" s="31" t="s">
+      <c r="AF1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="AG1" s="32" t="s">
+      <c r="AG1" s="34" t="s">
         <v>17</v>
       </c>
       <c r="AH1" s="14" t="s">
@@ -1544,19 +1581,19 @@
       </c>
     </row>
     <row r="2" spans="1:34">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="50" t="s">
         <v>29</v>
       </c>
       <c r="F2" s="7">
@@ -1568,7 +1605,7 @@
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="19"/>
-      <c r="K2" s="49" t="s">
+      <c r="K2" s="51" t="s">
         <v>29</v>
       </c>
       <c r="L2" s="21"/>
@@ -1588,17 +1625,17 @@
         <f t="shared" ref="Q2:Q37" si="0">P2+O2</f>
         <v>300</v>
       </c>
-      <c r="R2" s="35">
+      <c r="R2" s="37">
         <v>4.5161290322580597E-3</v>
       </c>
-      <c r="S2" s="36">
+      <c r="S2" s="38">
         <v>1.3548387096774199</v>
       </c>
       <c r="T2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="37"/>
-      <c r="V2" s="38">
+      <c r="U2" s="39"/>
+      <c r="V2" s="40">
         <v>300</v>
       </c>
       <c r="W2" s="23">
@@ -1608,17 +1645,17 @@
         <f t="shared" ref="X2:X37" si="1">W2+V2</f>
         <v>45300</v>
       </c>
-      <c r="Y2" s="35">
+      <c r="Y2" s="37">
         <v>3.1182795698924699E-3</v>
       </c>
-      <c r="Z2" s="36">
+      <c r="Z2" s="38">
         <v>141.258064516129</v>
       </c>
       <c r="AA2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="38">
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="40">
         <v>500</v>
       </c>
       <c r="AD2" s="23">
@@ -1628,10 +1665,10 @@
         <f t="shared" ref="AE2:AE37" si="2">AD2+AC2</f>
         <v>450500</v>
       </c>
-      <c r="AF2" s="35">
+      <c r="AF2" s="37">
         <v>2.7956989247311802E-3</v>
       </c>
-      <c r="AG2" s="36">
+      <c r="AG2" s="38">
         <v>1259.4623655913999</v>
       </c>
       <c r="AH2" s="19" t="s">
@@ -1639,19 +1676,19 @@
       </c>
     </row>
     <row r="3" spans="1:34">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="50" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="7">
@@ -1663,7 +1700,7 @@
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="19"/>
-      <c r="K3" s="49" t="s">
+      <c r="K3" s="51" t="s">
         <v>37</v>
       </c>
       <c r="L3" s="21"/>
@@ -1683,17 +1720,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R3" s="35">
+      <c r="R3" s="37">
         <v>1.11827956989247E-2</v>
       </c>
-      <c r="S3" s="36">
+      <c r="S3" s="38">
         <v>1.1182795698924699</v>
       </c>
       <c r="T3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U3" s="37"/>
-      <c r="V3" s="38">
+      <c r="U3" s="39"/>
+      <c r="V3" s="40">
         <v>100</v>
       </c>
       <c r="W3" s="23">
@@ -1703,17 +1740,17 @@
         <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="Y3" s="35">
+      <c r="Y3" s="37">
         <v>8.8172043010752692E-3</v>
       </c>
-      <c r="Z3" s="36">
+      <c r="Z3" s="38">
         <v>18.5161290322581</v>
       </c>
       <c r="AA3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="38">
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="40">
         <v>300</v>
       </c>
       <c r="AD3" s="23">
@@ -1723,10 +1760,10 @@
         <f t="shared" si="2"/>
         <v>20300</v>
       </c>
-      <c r="AF3" s="35">
+      <c r="AF3" s="37">
         <v>8.0645161290322596E-3</v>
       </c>
-      <c r="AG3" s="36">
+      <c r="AG3" s="38">
         <v>163.70967741935499</v>
       </c>
       <c r="AH3" s="19" t="s">
@@ -1734,19 +1771,19 @@
       </c>
     </row>
     <row r="4" spans="1:34">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="50" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="7">
@@ -1758,7 +1795,7 @@
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="19"/>
-      <c r="K4" s="49" t="s">
+      <c r="K4" s="51" t="s">
         <v>39</v>
       </c>
       <c r="L4" s="21" t="s">
@@ -1780,17 +1817,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R4" s="35">
+      <c r="R4" s="37">
         <v>0.103225806451613</v>
       </c>
-      <c r="S4" s="36">
+      <c r="S4" s="38">
         <v>10.322580645161301</v>
       </c>
       <c r="T4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="37"/>
-      <c r="V4" s="38">
+      <c r="U4" s="39"/>
+      <c r="V4" s="40">
         <v>100</v>
       </c>
       <c r="W4" s="23">
@@ -1800,17 +1837,17 @@
         <f t="shared" si="1"/>
         <v>3100</v>
       </c>
-      <c r="Y4" s="35">
+      <c r="Y4" s="37">
         <v>9.4623655913978505E-2</v>
       </c>
-      <c r="Z4" s="36">
+      <c r="Z4" s="38">
         <v>293.33333333333297</v>
       </c>
       <c r="AA4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB4" s="37"/>
-      <c r="AC4" s="38">
+      <c r="AB4" s="39"/>
+      <c r="AC4" s="40">
         <v>300</v>
       </c>
       <c r="AD4" s="23">
@@ -1820,10 +1857,10 @@
         <f t="shared" si="2"/>
         <v>30300</v>
       </c>
-      <c r="AF4" s="35">
+      <c r="AF4" s="37">
         <v>8.4946236559139798E-2</v>
       </c>
-      <c r="AG4" s="36">
+      <c r="AG4" s="38">
         <v>2573.8709677419401</v>
       </c>
       <c r="AH4" s="19" t="s">
@@ -1831,19 +1868,19 @@
       </c>
     </row>
     <row r="5" spans="1:34">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="50" t="s">
         <v>47</v>
       </c>
       <c r="F5" s="7">
@@ -1855,7 +1892,7 @@
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="19"/>
-      <c r="K5" s="49" t="s">
+      <c r="K5" s="51" t="s">
         <v>47</v>
       </c>
       <c r="L5" s="21" t="s">
@@ -1877,17 +1914,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R5" s="35">
+      <c r="R5" s="37">
         <v>4.5161290322580601E-2</v>
       </c>
-      <c r="S5" s="36">
+      <c r="S5" s="38">
         <v>4.5161290322580596</v>
       </c>
       <c r="T5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="37"/>
-      <c r="V5" s="38">
+      <c r="U5" s="39"/>
+      <c r="V5" s="40">
         <v>100</v>
       </c>
       <c r="W5" s="23">
@@ -1897,17 +1934,17 @@
         <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="Y5" s="35">
+      <c r="Y5" s="37">
         <v>3.5483870967741901E-2</v>
       </c>
-      <c r="Z5" s="36">
+      <c r="Z5" s="38">
         <v>74.516129032258107</v>
       </c>
       <c r="AA5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB5" s="37"/>
-      <c r="AC5" s="38">
+      <c r="AB5" s="39"/>
+      <c r="AC5" s="40">
         <v>300</v>
       </c>
       <c r="AD5" s="23">
@@ -1917,10 +1954,10 @@
         <f t="shared" si="2"/>
         <v>20300</v>
       </c>
-      <c r="AF5" s="35">
+      <c r="AF5" s="37">
         <v>3.2258064516128997E-2</v>
       </c>
-      <c r="AG5" s="36">
+      <c r="AG5" s="38">
         <v>654.83870967741905</v>
       </c>
       <c r="AH5" s="19" t="s">
@@ -1928,19 +1965,19 @@
       </c>
     </row>
     <row r="6" spans="1:34">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="50" t="s">
         <v>53</v>
       </c>
       <c r="F6" s="7">
@@ -1952,7 +1989,7 @@
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="49" t="s">
+      <c r="K6" s="51" t="s">
         <v>53</v>
       </c>
       <c r="L6" s="21" t="s">
@@ -1974,17 +2011,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R6" s="35">
+      <c r="R6" s="37">
         <v>1.50537634408602E-2</v>
       </c>
-      <c r="S6" s="36">
+      <c r="S6" s="38">
         <v>1.5053763440860199</v>
       </c>
       <c r="T6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U6" s="37"/>
-      <c r="V6" s="38">
+      <c r="U6" s="39"/>
+      <c r="V6" s="40">
         <v>100</v>
       </c>
       <c r="W6" s="23">
@@ -1994,17 +2031,17 @@
         <f t="shared" si="1"/>
         <v>4100</v>
       </c>
-      <c r="Y6" s="35">
+      <c r="Y6" s="37">
         <v>1.0752688172042999E-2</v>
       </c>
-      <c r="Z6" s="36">
+      <c r="Z6" s="38">
         <v>44.086021505376301</v>
       </c>
       <c r="AA6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB6" s="37"/>
-      <c r="AC6" s="38">
+      <c r="AB6" s="39"/>
+      <c r="AC6" s="40">
         <v>300</v>
       </c>
       <c r="AD6" s="23">
@@ -2014,10 +2051,10 @@
         <f t="shared" si="2"/>
         <v>40300</v>
       </c>
-      <c r="AF6" s="35">
+      <c r="AF6" s="37">
         <v>1.0322580645161301E-2</v>
       </c>
-      <c r="AG6" s="36">
+      <c r="AG6" s="38">
         <v>416</v>
       </c>
       <c r="AH6" s="19" t="s">
@@ -2025,19 +2062,19 @@
       </c>
     </row>
     <row r="7" spans="1:34">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="50" t="s">
         <v>59</v>
       </c>
       <c r="F7" s="7">
@@ -2049,7 +2086,7 @@
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="19"/>
-      <c r="K7" s="49" t="s">
+      <c r="K7" s="51" t="s">
         <v>59</v>
       </c>
       <c r="L7" s="21" t="s">
@@ -2071,17 +2108,17 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="R7" s="35">
+      <c r="R7" s="37">
         <v>5.0537634408602203</v>
       </c>
-      <c r="S7" s="36">
+      <c r="S7" s="38">
         <v>75.806451612903203</v>
       </c>
       <c r="T7" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="37"/>
-      <c r="V7" s="38">
+      <c r="U7" s="39"/>
+      <c r="V7" s="40">
         <v>10</v>
       </c>
       <c r="W7" s="23">
@@ -2091,17 +2128,17 @@
         <f t="shared" si="1"/>
         <v>2010</v>
       </c>
-      <c r="Y7" s="35">
+      <c r="Y7" s="37">
         <v>2.4731182795698898</v>
       </c>
-      <c r="Z7" s="36">
+      <c r="Z7" s="38">
         <v>4970.9677419354803</v>
       </c>
       <c r="AA7" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB7" s="37"/>
-      <c r="AC7" s="38">
+      <c r="AB7" s="39"/>
+      <c r="AC7" s="40">
         <v>50</v>
       </c>
       <c r="AD7" s="23">
@@ -2111,10 +2148,10 @@
         <f t="shared" si="2"/>
         <v>20050</v>
       </c>
-      <c r="AF7" s="35">
+      <c r="AF7" s="37">
         <v>1.2903225806451599</v>
       </c>
-      <c r="AG7" s="36">
+      <c r="AG7" s="38">
         <v>25870.967741935499</v>
       </c>
       <c r="AH7" s="19" t="s">
@@ -2122,19 +2159,19 @@
       </c>
     </row>
     <row r="8" spans="1:34">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="50" t="s">
         <v>66</v>
       </c>
       <c r="F8" s="7">
@@ -2146,7 +2183,7 @@
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="19"/>
-      <c r="K8" s="49" t="s">
+      <c r="K8" s="51" t="s">
         <v>66</v>
       </c>
       <c r="L8" s="21" t="s">
@@ -2168,17 +2205,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R8" s="35">
+      <c r="R8" s="37">
         <v>8.6021505376344107E-2</v>
       </c>
-      <c r="S8" s="36">
+      <c r="S8" s="38">
         <v>8.6021505376344098</v>
       </c>
       <c r="T8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U8" s="37"/>
-      <c r="V8" s="38">
+      <c r="U8" s="39"/>
+      <c r="V8" s="40">
         <v>100</v>
       </c>
       <c r="W8" s="23">
@@ -2188,17 +2225,17 @@
         <f t="shared" si="1"/>
         <v>5100</v>
       </c>
-      <c r="Y8" s="35">
+      <c r="Y8" s="37">
         <v>7.4193548387096797E-2</v>
       </c>
-      <c r="Z8" s="36">
+      <c r="Z8" s="38">
         <v>378.38709677419399</v>
       </c>
       <c r="AA8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB8" s="37"/>
-      <c r="AC8" s="38">
+      <c r="AB8" s="39"/>
+      <c r="AC8" s="40">
         <v>300</v>
       </c>
       <c r="AD8" s="23">
@@ -2208,10 +2245,10 @@
         <f t="shared" si="2"/>
         <v>50300</v>
       </c>
-      <c r="AF8" s="35">
+      <c r="AF8" s="37">
         <v>6.4516129032258104E-2</v>
       </c>
-      <c r="AG8" s="36">
+      <c r="AG8" s="38">
         <v>3245.16129032258</v>
       </c>
       <c r="AH8" s="19" t="s">
@@ -2219,19 +2256,19 @@
       </c>
     </row>
     <row r="9" spans="1:34">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="50" t="s">
         <v>71</v>
       </c>
       <c r="F9" s="7">
@@ -2243,7 +2280,7 @@
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="19"/>
-      <c r="K9" s="49" t="s">
+      <c r="K9" s="51" t="s">
         <v>71</v>
       </c>
       <c r="L9" s="21" t="s">
@@ -2265,17 +2302,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R9" s="35">
+      <c r="R9" s="37">
         <v>5.0537634408602199E-2</v>
       </c>
-      <c r="S9" s="36">
+      <c r="S9" s="38">
         <v>5.0537634408602203</v>
       </c>
       <c r="T9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U9" s="37"/>
-      <c r="V9" s="38">
+      <c r="U9" s="39"/>
+      <c r="V9" s="40">
         <v>100</v>
       </c>
       <c r="W9" s="23">
@@ -2285,17 +2322,17 @@
         <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="Y9" s="35">
+      <c r="Y9" s="37">
         <v>4.7311827956989197E-2</v>
       </c>
-      <c r="Z9" s="36">
+      <c r="Z9" s="38">
         <v>99.354838709677395</v>
       </c>
       <c r="AA9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB9" s="37"/>
-      <c r="AC9" s="38">
+      <c r="AB9" s="39"/>
+      <c r="AC9" s="40">
         <v>300</v>
       </c>
       <c r="AD9" s="23">
@@ -2305,10 +2342,10 @@
         <f t="shared" si="2"/>
         <v>20300</v>
       </c>
-      <c r="AF9" s="35">
+      <c r="AF9" s="37">
         <v>4.2473118279569899E-2</v>
       </c>
-      <c r="AG9" s="36">
+      <c r="AG9" s="38">
         <v>862.20430107526897</v>
       </c>
       <c r="AH9" s="19" t="s">
@@ -2316,19 +2353,19 @@
       </c>
     </row>
     <row r="10" spans="1:34">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="50" t="s">
         <v>78</v>
       </c>
       <c r="F10" s="7">
@@ -2340,7 +2377,7 @@
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="19"/>
-      <c r="K10" s="49" t="s">
+      <c r="K10" s="51" t="s">
         <v>78</v>
       </c>
       <c r="L10" s="21"/>
@@ -2358,17 +2395,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R10" s="35">
+      <c r="R10" s="37">
         <v>6.12903225806452E-2</v>
       </c>
-      <c r="S10" s="36">
+      <c r="S10" s="38">
         <v>6.1290322580645196</v>
       </c>
       <c r="T10" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U10" s="37"/>
-      <c r="V10" s="38">
+      <c r="U10" s="39"/>
+      <c r="V10" s="40">
         <v>100</v>
       </c>
       <c r="W10" s="23">
@@ -2378,17 +2415,17 @@
         <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="Y10" s="35">
+      <c r="Y10" s="37">
         <v>4.7311827956989197E-2</v>
       </c>
-      <c r="Z10" s="36">
+      <c r="Z10" s="38">
         <v>99.354838709677395</v>
       </c>
       <c r="AA10" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB10" s="37"/>
-      <c r="AC10" s="38">
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="40">
         <v>300</v>
       </c>
       <c r="AD10" s="23">
@@ -2398,10 +2435,10 @@
         <f t="shared" si="2"/>
         <v>20300</v>
       </c>
-      <c r="AF10" s="40">
+      <c r="AF10" s="42">
         <v>3.7311827956989299E-2</v>
       </c>
-      <c r="AG10" s="36">
+      <c r="AG10" s="38">
         <v>757.43010752688201</v>
       </c>
       <c r="AH10" s="19" t="s">
@@ -2409,19 +2446,19 @@
       </c>
     </row>
     <row r="11" spans="1:34">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="50" t="s">
         <v>82</v>
       </c>
       <c r="F11" s="7">
@@ -2433,7 +2470,7 @@
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="19"/>
-      <c r="K11" s="49" t="s">
+      <c r="K11" s="51" t="s">
         <v>82</v>
       </c>
       <c r="L11" s="21" t="s">
@@ -2455,17 +2492,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R11" s="35">
+      <c r="R11" s="37">
         <v>0.138709677419355</v>
       </c>
-      <c r="S11" s="36">
+      <c r="S11" s="38">
         <v>13.8709677419355</v>
       </c>
       <c r="T11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U11" s="37"/>
-      <c r="V11" s="38">
+      <c r="U11" s="39"/>
+      <c r="V11" s="40">
         <v>100</v>
       </c>
       <c r="W11" s="23">
@@ -2475,17 +2512,17 @@
         <f t="shared" si="1"/>
         <v>4100</v>
       </c>
-      <c r="Y11" s="35">
+      <c r="Y11" s="37">
         <v>9.4623655913978505E-2</v>
       </c>
-      <c r="Z11" s="36">
+      <c r="Z11" s="38">
         <v>387.95698924731198</v>
       </c>
       <c r="AA11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB11" s="37"/>
-      <c r="AC11" s="38">
+      <c r="AB11" s="39"/>
+      <c r="AC11" s="40">
         <v>300</v>
       </c>
       <c r="AD11" s="23">
@@ -2495,10 +2532,10 @@
         <f t="shared" si="2"/>
         <v>40300</v>
       </c>
-      <c r="AF11" s="40">
+      <c r="AF11" s="42">
         <v>8.8172043010752696E-2</v>
       </c>
-      <c r="AG11" s="36">
+      <c r="AG11" s="38">
         <v>3553.3333333333298</v>
       </c>
       <c r="AH11" s="19" t="s">
@@ -2506,19 +2543,19 @@
       </c>
     </row>
     <row r="12" spans="1:34">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="50" t="s">
         <v>87</v>
       </c>
       <c r="F12" s="7">
@@ -2530,7 +2567,7 @@
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="19"/>
-      <c r="K12" s="49" t="s">
+      <c r="K12" s="51" t="s">
         <v>87</v>
       </c>
       <c r="L12" s="21" t="s">
@@ -2552,70 +2589,70 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R12" s="35">
+      <c r="R12" s="37">
         <v>16.989247311827999</v>
       </c>
-      <c r="S12" s="36">
+      <c r="S12" s="38">
         <v>84.946236559139805</v>
       </c>
       <c r="T12" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U12" s="37"/>
-      <c r="V12" s="39">
+      <c r="U12" s="39"/>
+      <c r="V12" s="41">
         <v>2</v>
       </c>
-      <c r="W12" s="28">
+      <c r="W12" s="29">
         <v>1000</v>
       </c>
-      <c r="X12" s="28">
+      <c r="X12" s="29">
         <f t="shared" si="1"/>
         <v>1002</v>
       </c>
-      <c r="Y12" s="40">
+      <c r="Y12" s="42">
         <v>14.623655913978499</v>
       </c>
-      <c r="Z12" s="36">
+      <c r="Z12" s="38">
         <v>14652.9032258065</v>
       </c>
-      <c r="AA12" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB12" s="41"/>
-      <c r="AC12" s="39">
+      <c r="AA12" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="41">
         <v>5</v>
       </c>
-      <c r="AD12" s="28">
+      <c r="AD12" s="29">
         <v>10000</v>
       </c>
-      <c r="AE12" s="28">
+      <c r="AE12" s="29">
         <f t="shared" si="2"/>
         <v>10005</v>
       </c>
-      <c r="AF12" s="40">
+      <c r="AF12" s="42">
         <v>13.9784946236559</v>
       </c>
-      <c r="AG12" s="36">
+      <c r="AG12" s="38">
         <v>139854.83870967699</v>
       </c>
-      <c r="AH12" s="25" t="s">
+      <c r="AH12" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:34">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="48" t="s">
+      <c r="E13" s="50" t="s">
         <v>94</v>
       </c>
       <c r="F13" s="7">
@@ -2627,7 +2664,7 @@
       </c>
       <c r="I13" s="18"/>
       <c r="J13" s="19"/>
-      <c r="K13" s="49" t="s">
+      <c r="K13" s="51" t="s">
         <v>94</v>
       </c>
       <c r="L13" s="21"/>
@@ -2645,37 +2682,37 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R13" s="35">
+      <c r="R13" s="37">
         <v>2.3655913978494598</v>
       </c>
-      <c r="S13" s="36">
+      <c r="S13" s="38">
         <v>11.8279569892473</v>
       </c>
       <c r="T13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U13" s="37"/>
-      <c r="V13" s="39">
+      <c r="U13" s="39"/>
+      <c r="V13" s="41">
         <v>10</v>
       </c>
-      <c r="W13" s="28">
+      <c r="W13" s="29">
         <v>1000</v>
       </c>
-      <c r="X13" s="28">
+      <c r="X13" s="29">
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-      <c r="Y13" s="40">
+      <c r="Y13" s="42">
         <v>1.1827956989247299</v>
       </c>
-      <c r="Z13" s="36">
+      <c r="Z13" s="38">
         <v>1194.62365591398</v>
       </c>
-      <c r="AA13" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB13" s="41"/>
-      <c r="AC13" s="39">
+      <c r="AA13" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB13" s="43"/>
+      <c r="AC13" s="41">
         <v>20</v>
       </c>
       <c r="AD13" s="23">
@@ -2685,30 +2722,30 @@
         <f t="shared" si="2"/>
         <v>10020</v>
       </c>
-      <c r="AF13" s="40">
+      <c r="AF13" s="42">
         <v>1.0752688172042999</v>
       </c>
-      <c r="AG13" s="36">
+      <c r="AG13" s="38">
         <v>10774.1935483871</v>
       </c>
-      <c r="AH13" s="25" t="s">
+      <c r="AH13" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:34">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="50" t="s">
         <v>97</v>
       </c>
       <c r="F14" s="7">
@@ -2720,7 +2757,7 @@
       </c>
       <c r="I14" s="18"/>
       <c r="J14" s="19"/>
-      <c r="K14" s="49" t="s">
+      <c r="K14" s="51" t="s">
         <v>97</v>
       </c>
       <c r="L14" s="21" t="s">
@@ -2742,17 +2779,17 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R14" s="35">
+      <c r="R14" s="37">
         <v>3.97849462365591</v>
       </c>
-      <c r="S14" s="36">
+      <c r="S14" s="38">
         <v>19.8924731182796</v>
       </c>
       <c r="T14" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="U14" s="37"/>
-      <c r="V14" s="38">
+      <c r="U14" s="39"/>
+      <c r="V14" s="40">
         <v>10</v>
       </c>
       <c r="W14" s="23">
@@ -2762,50 +2799,50 @@
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-      <c r="Y14" s="40">
+      <c r="Y14" s="42">
         <v>1.9892473118279601</v>
       </c>
-      <c r="Z14" s="36">
+      <c r="Z14" s="38">
         <v>2009.1397849462401</v>
       </c>
-      <c r="AA14" s="25" t="s">
+      <c r="AA14" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="AB14" s="41"/>
-      <c r="AC14" s="39">
+      <c r="AB14" s="43"/>
+      <c r="AC14" s="41">
         <v>10</v>
       </c>
-      <c r="AD14" s="28">
+      <c r="AD14" s="29">
         <v>10000</v>
       </c>
-      <c r="AE14" s="28">
+      <c r="AE14" s="29">
         <f t="shared" si="2"/>
         <v>10010</v>
       </c>
-      <c r="AF14" s="40">
+      <c r="AF14" s="42">
         <v>1.93548387096774</v>
       </c>
-      <c r="AG14" s="36">
+      <c r="AG14" s="38">
         <v>19374.193548387098</v>
       </c>
-      <c r="AH14" s="25" t="s">
+      <c r="AH14" s="32" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:34">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="50" t="s">
         <v>105</v>
       </c>
       <c r="F15" s="7">
@@ -2817,7 +2854,7 @@
       </c>
       <c r="I15" s="18"/>
       <c r="J15" s="19"/>
-      <c r="K15" s="49" t="s">
+      <c r="K15" s="51" t="s">
         <v>105</v>
       </c>
       <c r="L15" s="21" t="s">
@@ -2839,17 +2876,17 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="R15" s="35">
+      <c r="R15" s="37">
         <v>4.3010752688171996</v>
       </c>
-      <c r="S15" s="36">
+      <c r="S15" s="38">
         <v>43.010752688171998</v>
       </c>
       <c r="T15" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U15" s="37"/>
-      <c r="V15" s="38">
+      <c r="U15" s="39"/>
+      <c r="V15" s="40">
         <v>10</v>
       </c>
       <c r="W15" s="23">
@@ -2859,50 +2896,50 @@
         <f t="shared" si="1"/>
         <v>2010</v>
       </c>
-      <c r="Y15" s="40">
+      <c r="Y15" s="42">
         <v>3.76344086021505</v>
       </c>
-      <c r="Z15" s="36">
+      <c r="Z15" s="38">
         <v>7564.5161290322603</v>
       </c>
-      <c r="AA15" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB15" s="41"/>
-      <c r="AC15" s="39">
+      <c r="AA15" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB15" s="43"/>
+      <c r="AC15" s="41">
         <v>20</v>
       </c>
-      <c r="AD15" s="28">
+      <c r="AD15" s="29">
         <v>20000</v>
       </c>
-      <c r="AE15" s="28">
+      <c r="AE15" s="29">
         <f t="shared" si="2"/>
         <v>20020</v>
       </c>
-      <c r="AF15" s="40">
+      <c r="AF15" s="42">
         <v>3.54838709677419</v>
       </c>
-      <c r="AG15" s="36">
+      <c r="AG15" s="38">
         <v>71038.709677419305</v>
       </c>
-      <c r="AH15" s="25" t="s">
+      <c r="AH15" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="15">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="50" t="s">
         <v>110</v>
       </c>
       <c r="F16" s="7">
@@ -2916,7 +2953,7 @@
         <v>111</v>
       </c>
       <c r="J16" s="19"/>
-      <c r="K16" s="49" t="s">
+      <c r="K16" s="51" t="s">
         <v>110</v>
       </c>
       <c r="L16" s="21" t="s">
@@ -2938,70 +2975,70 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R16" s="40">
+      <c r="R16" s="42">
         <v>28.494623655914001</v>
       </c>
-      <c r="S16" s="36">
+      <c r="S16" s="38">
         <v>142.47311827957</v>
       </c>
       <c r="T16" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="41"/>
-      <c r="V16" s="39">
+      <c r="U16" s="43"/>
+      <c r="V16" s="41">
         <v>2</v>
       </c>
-      <c r="W16" s="28">
+      <c r="W16" s="29">
         <v>1000</v>
       </c>
-      <c r="X16" s="28">
+      <c r="X16" s="29">
         <f t="shared" si="1"/>
         <v>1002</v>
       </c>
-      <c r="Y16" s="40">
+      <c r="Y16" s="42">
         <v>21.290322580645199</v>
       </c>
-      <c r="Z16" s="36">
+      <c r="Z16" s="38">
         <v>21332.903225806502</v>
       </c>
-      <c r="AA16" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB16" s="41"/>
-      <c r="AC16" s="39">
+      <c r="AA16" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB16" s="43"/>
+      <c r="AC16" s="41">
         <v>5</v>
       </c>
-      <c r="AD16" s="28">
+      <c r="AD16" s="29">
         <v>10000</v>
       </c>
-      <c r="AE16" s="28">
+      <c r="AE16" s="29">
         <f t="shared" si="2"/>
         <v>10005</v>
       </c>
-      <c r="AF16" s="35">
+      <c r="AF16" s="37">
         <v>19.354838709677399</v>
       </c>
-      <c r="AG16" s="36">
+      <c r="AG16" s="38">
         <v>193645.16129032301</v>
       </c>
-      <c r="AH16" s="25" t="s">
+      <c r="AH16" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:34" s="2" customFormat="1" ht="15">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D17" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="50" t="s">
+      <c r="E17" s="52" t="s">
         <v>116</v>
       </c>
       <c r="F17" s="9">
@@ -3014,82 +3051,94 @@
       <c r="I17" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="J17" s="25"/>
-      <c r="K17" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="L17" s="26"/>
-      <c r="M17" s="27" t="s">
+      <c r="J17" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="N17" s="27" t="s">
+      <c r="K17" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="L17" s="27"/>
+      <c r="M17" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="N17" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="O17" s="28">
+      <c r="O17" s="29">
         <v>0</v>
       </c>
-      <c r="P17" s="28">
+      <c r="P17" s="29">
         <v>5</v>
       </c>
-      <c r="Q17" s="28">
+      <c r="Q17" s="29">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R17" s="40">
-        <v>0</v>
-      </c>
-      <c r="S17" s="36">
-        <v>0</v>
-      </c>
-      <c r="T17" s="25"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="39"/>
-      <c r="W17" s="28">
+      <c r="R17" s="42">
+        <v>2.8</v>
+      </c>
+      <c r="S17" s="38">
+        <v>14</v>
+      </c>
+      <c r="T17" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="U17" s="43"/>
+      <c r="V17" s="41">
+        <v>10</v>
+      </c>
+      <c r="W17" s="29">
         <v>1000</v>
       </c>
-      <c r="X17" s="28">
+      <c r="X17" s="29">
         <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="Y17" s="40">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="25"/>
-      <c r="AB17" s="41"/>
-      <c r="AC17" s="39"/>
-      <c r="AD17" s="28">
+        <v>1010</v>
+      </c>
+      <c r="Y17" s="42">
+        <v>1.6667000000000001</v>
+      </c>
+      <c r="Z17" s="38">
+        <v>1683.367</v>
+      </c>
+      <c r="AA17" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB17" s="43"/>
+      <c r="AC17" s="41">
+        <v>20</v>
+      </c>
+      <c r="AD17" s="29">
         <v>10000</v>
       </c>
-      <c r="AE17" s="28">
+      <c r="AE17" s="29">
         <f t="shared" si="2"/>
-        <v>10000</v>
-      </c>
-      <c r="AF17" s="40">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="36">
-        <v>0</v>
-      </c>
-      <c r="AH17" s="27"/>
+        <v>10020</v>
+      </c>
+      <c r="AF17" s="42">
+        <v>1.45161290322581</v>
+      </c>
+      <c r="AG17" s="38">
+        <v>14545.1612903226</v>
+      </c>
+      <c r="AH17" s="28" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="1:34" ht="15">
-      <c r="A18" s="48" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="48" t="s">
+      <c r="A18" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" s="48" t="s">
-        <v>121</v>
+      <c r="B18" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>123</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
@@ -3101,13 +3150,15 @@
       <c r="I18" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="49" t="s">
-        <v>121</v>
+      <c r="J18" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>126</v>
       </c>
       <c r="L18" s="21"/>
       <c r="M18" s="22" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="N18" s="22" t="s">
         <v>32</v>
@@ -3122,15 +3173,17 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R18" s="35">
-        <v>0</v>
-      </c>
-      <c r="S18" s="36">
-        <v>0</v>
-      </c>
-      <c r="T18" s="19"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="38"/>
+      <c r="R18" s="37">
+        <v>98.4</v>
+      </c>
+      <c r="S18" s="38">
+        <v>492</v>
+      </c>
+      <c r="T18" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="U18" s="39"/>
+      <c r="V18" s="40"/>
       <c r="W18" s="23">
         <v>1000</v>
       </c>
@@ -3138,15 +3191,17 @@
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="Y18" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="37"/>
-      <c r="AC18" s="38"/>
+      <c r="Y18" s="37">
+        <v>43.548387096774199</v>
+      </c>
+      <c r="Z18" s="38">
+        <v>43548.387096774197</v>
+      </c>
+      <c r="AA18" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB18" s="39"/>
+      <c r="AC18" s="40"/>
       <c r="AD18" s="23">
         <v>10000</v>
       </c>
@@ -3154,29 +3209,31 @@
         <f t="shared" si="2"/>
         <v>10000</v>
       </c>
-      <c r="AF18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="36">
-        <v>0</v>
-      </c>
-      <c r="AH18" s="22"/>
+      <c r="AF18" s="37">
+        <v>43.010752688171998</v>
+      </c>
+      <c r="AG18" s="38">
+        <v>430107.52688172</v>
+      </c>
+      <c r="AH18" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="19" spans="1:34">
-      <c r="A19" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" s="48" t="s">
-        <v>125</v>
+      <c r="A19" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="50" t="s">
+        <v>130</v>
       </c>
       <c r="F19" s="7">
         <v>1</v>
@@ -3186,13 +3243,15 @@
         <v>30</v>
       </c>
       <c r="I19" s="18"/>
-      <c r="J19" s="19"/>
+      <c r="J19" s="25" t="s">
+        <v>132</v>
+      </c>
       <c r="K19" s="20" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="L19" s="21"/>
       <c r="M19" s="22" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="N19" s="22" t="s">
         <v>32</v>
@@ -3207,17 +3266,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R19" s="35">
-        <v>0.50537634408602194</v>
-      </c>
-      <c r="S19" s="36">
-        <v>2.5268817204301102</v>
-      </c>
-      <c r="T19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="U19" s="37"/>
-      <c r="V19" s="38">
+      <c r="R19" s="37"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="39"/>
+      <c r="V19" s="40">
         <v>5</v>
       </c>
       <c r="W19" s="23">
@@ -3227,17 +3280,11 @@
         <f t="shared" si="1"/>
         <v>1005</v>
       </c>
-      <c r="Y19" s="35">
-        <v>0.32258064516128998</v>
-      </c>
-      <c r="Z19" s="36">
-        <v>324.193548387097</v>
-      </c>
-      <c r="AA19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB19" s="37"/>
-      <c r="AC19" s="38">
+      <c r="Y19" s="37"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="39"/>
+      <c r="AC19" s="40">
         <v>10</v>
       </c>
       <c r="AD19" s="23">
@@ -3247,31 +3294,25 @@
         <f t="shared" si="2"/>
         <v>10010</v>
       </c>
-      <c r="AF19" s="35">
-        <v>0.30107526881720398</v>
-      </c>
-      <c r="AG19" s="36">
-        <v>3013.7634408602198</v>
-      </c>
-      <c r="AH19" s="19" t="s">
-        <v>33</v>
-      </c>
+      <c r="AF19" s="37"/>
+      <c r="AG19" s="38"/>
+      <c r="AH19" s="19"/>
     </row>
     <row r="20" spans="1:34" ht="15">
-      <c r="A20" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" s="48" t="s">
-        <v>130</v>
+      <c r="A20" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>136</v>
       </c>
       <c r="F20" s="7">
         <v>1</v>
@@ -3281,15 +3322,17 @@
         <v>30</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="29" t="s">
-        <v>133</v>
+        <v>138</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="K20" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="22" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="N20" s="22" t="s">
         <v>32</v>
@@ -3304,17 +3347,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R20" s="35">
-        <v>0.59139784946236595</v>
-      </c>
-      <c r="S20" s="36">
-        <v>2.9569892473118302</v>
-      </c>
-      <c r="T20" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="U20" s="37"/>
-      <c r="V20" s="38">
+      <c r="R20" s="37"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="39"/>
+      <c r="V20" s="40">
         <v>5</v>
       </c>
       <c r="W20" s="23">
@@ -3324,17 +3361,11 @@
         <f t="shared" si="1"/>
         <v>1005</v>
       </c>
-      <c r="Y20" s="35">
-        <v>0.36559139784946199</v>
-      </c>
-      <c r="Z20" s="36">
-        <v>367.41935483870998</v>
-      </c>
-      <c r="AA20" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB20" s="37"/>
-      <c r="AC20" s="38">
+      <c r="Y20" s="37"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="39"/>
+      <c r="AC20" s="40">
         <v>10</v>
       </c>
       <c r="AD20" s="23">
@@ -3344,31 +3375,25 @@
         <f t="shared" si="2"/>
         <v>10010</v>
       </c>
-      <c r="AF20" s="35">
-        <v>0.31182795698924698</v>
-      </c>
-      <c r="AG20" s="36">
-        <v>3121.3978494623698</v>
-      </c>
-      <c r="AH20" s="19" t="s">
-        <v>33</v>
-      </c>
+      <c r="AF20" s="37"/>
+      <c r="AG20" s="38"/>
+      <c r="AH20" s="19"/>
     </row>
     <row r="21" spans="1:34">
-      <c r="A21" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="B21" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="E21" s="48" t="s">
-        <v>139</v>
+      <c r="A21" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>146</v>
       </c>
       <c r="F21" s="7">
         <v>2</v>
@@ -3379,17 +3404,17 @@
       </c>
       <c r="I21" s="18"/>
       <c r="J21" s="19"/>
-      <c r="K21" s="49" t="s">
-        <v>139</v>
+      <c r="K21" s="51" t="s">
+        <v>146</v>
       </c>
       <c r="L21" s="21" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="M21" s="22" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="N21" s="22" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="O21" s="23">
         <v>0</v>
@@ -3401,17 +3426,17 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="R21" s="35">
+      <c r="R21" s="37">
         <v>2.6881720430107499</v>
       </c>
-      <c r="S21" s="36">
+      <c r="S21" s="38">
         <v>26.881720430107499</v>
       </c>
       <c r="T21" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="U21" s="37"/>
-      <c r="V21" s="38">
+      <c r="U21" s="39"/>
+      <c r="V21" s="40">
         <v>10</v>
       </c>
       <c r="W21" s="23">
@@ -3421,17 +3446,17 @@
         <f t="shared" si="1"/>
         <v>2010</v>
       </c>
-      <c r="Y21" s="35">
+      <c r="Y21" s="37">
         <v>1.72043010752688</v>
       </c>
-      <c r="Z21" s="36">
+      <c r="Z21" s="38">
         <v>3458.0645161290299</v>
       </c>
       <c r="AA21" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="AB21" s="37"/>
-      <c r="AC21" s="38">
+      <c r="AB21" s="39"/>
+      <c r="AC21" s="40">
         <v>20</v>
       </c>
       <c r="AD21" s="23">
@@ -3441,29 +3466,29 @@
         <f t="shared" si="2"/>
         <v>20020</v>
       </c>
-      <c r="AF21" s="35">
+      <c r="AF21" s="37">
         <v>1.1827956989247299</v>
       </c>
-      <c r="AG21" s="36">
+      <c r="AG21" s="38">
         <v>23679.5698924731</v>
       </c>
       <c r="AH21" s="22" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:34">
-      <c r="A22" s="48" t="s">
-        <v>144</v>
+      <c r="A22" s="50" t="s">
+        <v>151</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="D22" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="E22" s="48" t="s">
-        <v>147</v>
+      <c r="C22" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>154</v>
       </c>
       <c r="F22" s="7">
         <v>1</v>
@@ -3474,14 +3499,14 @@
       </c>
       <c r="I22" s="18"/>
       <c r="J22" s="19"/>
-      <c r="K22" s="49" t="s">
-        <v>147</v>
+      <c r="K22" s="51" t="s">
+        <v>154</v>
       </c>
       <c r="L22" s="21" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="M22" s="22" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="N22" s="22" t="s">
         <v>43</v>
@@ -3496,17 +3521,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R22" s="35">
+      <c r="R22" s="37">
         <v>9.9051612903225797E-2</v>
       </c>
-      <c r="S22" s="36">
+      <c r="S22" s="38">
         <v>9.9051612903225799</v>
       </c>
       <c r="T22" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U22" s="37"/>
-      <c r="V22" s="38">
+      <c r="U22" s="39"/>
+      <c r="V22" s="40">
         <v>100</v>
       </c>
       <c r="W22" s="23">
@@ -3516,17 +3541,17 @@
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
-      <c r="Y22" s="35">
+      <c r="Y22" s="37">
         <v>7.6821505376344107E-2</v>
       </c>
-      <c r="Z22" s="36">
+      <c r="Z22" s="38">
         <v>84.503655913978506</v>
       </c>
       <c r="AA22" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB22" s="37"/>
-      <c r="AC22" s="38">
+      <c r="AB22" s="39"/>
+      <c r="AC22" s="40">
         <v>200</v>
       </c>
       <c r="AD22" s="23">
@@ -3536,10 +3561,10 @@
         <f t="shared" si="2"/>
         <v>10200</v>
       </c>
-      <c r="AF22" s="35">
+      <c r="AF22" s="37">
         <v>5.9531182795698898E-2</v>
       </c>
-      <c r="AG22" s="36">
+      <c r="AG22" s="38">
         <v>607.21806451612895</v>
       </c>
       <c r="AH22" s="19" t="s">
@@ -3547,20 +3572,20 @@
       </c>
     </row>
     <row r="23" spans="1:34">
-      <c r="A23" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="D23" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="E23" s="48" t="s">
-        <v>147</v>
+      <c r="A23" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="50" t="s">
+        <v>154</v>
       </c>
       <c r="F23" s="7">
         <v>1</v>
@@ -3571,14 +3596,14 @@
       </c>
       <c r="I23" s="18"/>
       <c r="J23" s="19"/>
-      <c r="K23" s="49" t="s">
-        <v>147</v>
+      <c r="K23" s="51" t="s">
+        <v>154</v>
       </c>
       <c r="L23" s="21" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="N23" s="22" t="s">
         <v>43</v>
@@ -3593,17 +3618,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R23" s="35">
+      <c r="R23" s="37">
         <v>9.9051612903225797E-2</v>
       </c>
-      <c r="S23" s="36">
+      <c r="S23" s="38">
         <v>9.9051612903225799</v>
       </c>
       <c r="T23" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U23" s="37"/>
-      <c r="V23" s="38">
+      <c r="U23" s="39"/>
+      <c r="V23" s="40">
         <v>100</v>
       </c>
       <c r="W23" s="23">
@@ -3613,17 +3638,17 @@
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
-      <c r="Y23" s="35">
+      <c r="Y23" s="37">
         <v>7.6821505376344107E-2</v>
       </c>
-      <c r="Z23" s="36">
+      <c r="Z23" s="38">
         <v>84.503655913978506</v>
       </c>
       <c r="AA23" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB23" s="37"/>
-      <c r="AC23" s="38">
+      <c r="AB23" s="39"/>
+      <c r="AC23" s="40">
         <v>200</v>
       </c>
       <c r="AD23" s="23">
@@ -3633,10 +3658,10 @@
         <f t="shared" si="2"/>
         <v>10200</v>
       </c>
-      <c r="AF23" s="35">
+      <c r="AF23" s="37">
         <v>5.9531182795698898E-2</v>
       </c>
-      <c r="AG23" s="36">
+      <c r="AG23" s="38">
         <v>607.21806451612895</v>
       </c>
       <c r="AH23" s="19" t="s">
@@ -3644,20 +3669,20 @@
       </c>
     </row>
     <row r="24" spans="1:34">
-      <c r="A24" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="D24" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="E24" s="48" t="s">
-        <v>155</v>
+      <c r="A24" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>162</v>
       </c>
       <c r="F24" s="7">
         <v>14</v>
@@ -3668,17 +3693,17 @@
       </c>
       <c r="I24" s="18"/>
       <c r="J24" s="19"/>
-      <c r="K24" s="49" t="s">
-        <v>155</v>
+      <c r="K24" s="51" t="s">
+        <v>162</v>
       </c>
       <c r="L24" s="21" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="M24" s="22" t="s">
         <v>31</v>
       </c>
       <c r="N24" s="22" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="O24" s="23">
         <v>130</v>
@@ -3690,17 +3715,17 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="R24" s="35">
+      <c r="R24" s="37">
         <v>2.4731182795698901E-3</v>
       </c>
-      <c r="S24" s="36">
+      <c r="S24" s="38">
         <v>0.494623655913978</v>
       </c>
       <c r="T24" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U24" s="37"/>
-      <c r="V24" s="38">
+      <c r="U24" s="39"/>
+      <c r="V24" s="40">
         <v>200</v>
       </c>
       <c r="W24" s="23">
@@ -3710,17 +3735,17 @@
         <f t="shared" si="1"/>
         <v>14200</v>
       </c>
-      <c r="Y24" s="35">
+      <c r="Y24" s="37">
         <v>1.8279569892473101E-3</v>
       </c>
-      <c r="Z24" s="36">
+      <c r="Z24" s="38">
         <v>25.9569892473118</v>
       </c>
       <c r="AA24" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB24" s="37"/>
-      <c r="AC24" s="38">
+      <c r="AB24" s="39"/>
+      <c r="AC24" s="40">
         <v>300</v>
       </c>
       <c r="AD24" s="23">
@@ -3730,10 +3755,10 @@
         <f t="shared" si="2"/>
         <v>140300</v>
       </c>
-      <c r="AF24" s="35">
+      <c r="AF24" s="37">
         <v>1.72043010752688E-3</v>
       </c>
-      <c r="AG24" s="36">
+      <c r="AG24" s="38">
         <v>241.37634408602199</v>
       </c>
       <c r="AH24" s="19" t="s">
@@ -3741,20 +3766,20 @@
       </c>
     </row>
     <row r="25" spans="1:34">
-      <c r="A25" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="D25" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="E25" s="48" t="s">
+      <c r="A25" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" s="50" t="s">
         <v>161</v>
+      </c>
+      <c r="E25" s="50" t="s">
+        <v>168</v>
       </c>
       <c r="F25" s="7">
         <v>2</v>
@@ -3765,17 +3790,17 @@
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="19"/>
-      <c r="K25" s="49" t="s">
-        <v>161</v>
+      <c r="K25" s="51" t="s">
+        <v>168</v>
       </c>
       <c r="L25" s="21" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="M25" s="22" t="s">
         <v>31</v>
       </c>
       <c r="N25" s="22" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="O25" s="23">
         <v>90</v>
@@ -3787,17 +3812,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R25" s="35">
+      <c r="R25" s="37">
         <v>2.7956989247311802E-3</v>
       </c>
-      <c r="S25" s="36">
+      <c r="S25" s="38">
         <v>0.27956989247311798</v>
       </c>
       <c r="T25" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U25" s="37"/>
-      <c r="V25" s="38">
+      <c r="U25" s="39"/>
+      <c r="V25" s="40">
         <v>100</v>
       </c>
       <c r="W25" s="23">
@@ -3807,17 +3832,17 @@
         <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="Y25" s="35">
+      <c r="Y25" s="37">
         <v>2.2580645161290299E-3</v>
       </c>
-      <c r="Z25" s="36">
+      <c r="Z25" s="38">
         <v>4.7419354838709697</v>
       </c>
       <c r="AA25" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB25" s="37"/>
-      <c r="AC25" s="38">
+      <c r="AB25" s="39"/>
+      <c r="AC25" s="40">
         <v>300</v>
       </c>
       <c r="AD25" s="23">
@@ -3827,10 +3852,10 @@
         <f t="shared" si="2"/>
         <v>20300</v>
       </c>
-      <c r="AF25" s="35">
+      <c r="AF25" s="37">
         <v>1.93548387096774E-3</v>
       </c>
-      <c r="AG25" s="36">
+      <c r="AG25" s="38">
         <v>39.290322580645203</v>
       </c>
       <c r="AH25" s="19" t="s">
@@ -3838,20 +3863,20 @@
       </c>
     </row>
     <row r="26" spans="1:34">
-      <c r="A26" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>164</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="D26" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="E26" s="48" t="s">
-        <v>167</v>
+      <c r="A26" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" s="50" t="s">
+        <v>174</v>
       </c>
       <c r="F26" s="7">
         <v>2</v>
@@ -3862,11 +3887,11 @@
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="19"/>
-      <c r="K26" s="49" t="s">
-        <v>167</v>
+      <c r="K26" s="51" t="s">
+        <v>174</v>
       </c>
       <c r="L26" s="21" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="M26" s="22" t="s">
         <v>31</v>
@@ -3884,17 +3909,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R26" s="35">
+      <c r="R26" s="37">
         <v>5.4838709677419396E-3</v>
       </c>
-      <c r="S26" s="36">
+      <c r="S26" s="38">
         <v>0.54838709677419395</v>
       </c>
       <c r="T26" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U26" s="37"/>
-      <c r="V26" s="38">
+      <c r="U26" s="39"/>
+      <c r="V26" s="40">
         <v>100</v>
       </c>
       <c r="W26" s="23">
@@ -3904,17 +3929,17 @@
         <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="Y26" s="35">
+      <c r="Y26" s="37">
         <v>4.3010752688172E-3</v>
       </c>
-      <c r="Z26" s="36">
+      <c r="Z26" s="38">
         <v>9.0322580645161299</v>
       </c>
       <c r="AA26" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB26" s="37"/>
-      <c r="AC26" s="38">
+      <c r="AB26" s="39"/>
+      <c r="AC26" s="40">
         <v>300</v>
       </c>
       <c r="AD26" s="23">
@@ -3924,10 +3949,10 @@
         <f t="shared" si="2"/>
         <v>20300</v>
       </c>
-      <c r="AF26" s="35">
+      <c r="AF26" s="37">
         <v>3.87096774193548E-3</v>
       </c>
-      <c r="AG26" s="36">
+      <c r="AG26" s="38">
         <v>78.580645161290306</v>
       </c>
       <c r="AH26" s="19" t="s">
@@ -3935,20 +3960,20 @@
       </c>
     </row>
     <row r="27" spans="1:34">
-      <c r="A27" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="B27" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="C27" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="D27" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="E27" s="48" t="s">
-        <v>172</v>
+      <c r="A27" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" s="50" t="s">
+        <v>179</v>
       </c>
       <c r="F27" s="7">
         <v>1</v>
@@ -3959,11 +3984,11 @@
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="19"/>
-      <c r="K27" s="49" t="s">
-        <v>172</v>
+      <c r="K27" s="51" t="s">
+        <v>179</v>
       </c>
       <c r="L27" s="21" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="M27" s="22" t="s">
         <v>31</v>
@@ -3981,17 +4006,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R27" s="35">
+      <c r="R27" s="37">
         <v>5.4838709677419396E-3</v>
       </c>
-      <c r="S27" s="36">
+      <c r="S27" s="38">
         <v>0.54838709677419395</v>
       </c>
       <c r="T27" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U27" s="37"/>
-      <c r="V27" s="38">
+      <c r="U27" s="39"/>
+      <c r="V27" s="40">
         <v>100</v>
       </c>
       <c r="W27" s="23">
@@ -4001,17 +4026,17 @@
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
-      <c r="Y27" s="35">
+      <c r="Y27" s="37">
         <v>4.3010752688172E-3</v>
       </c>
-      <c r="Z27" s="36">
+      <c r="Z27" s="38">
         <v>4.7311827956989196</v>
       </c>
       <c r="AA27" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB27" s="37"/>
-      <c r="AC27" s="38">
+      <c r="AB27" s="39"/>
+      <c r="AC27" s="40">
         <v>300</v>
       </c>
       <c r="AD27" s="23">
@@ -4021,10 +4046,10 @@
         <f t="shared" si="2"/>
         <v>10300</v>
       </c>
-      <c r="AF27" s="35">
+      <c r="AF27" s="37">
         <v>3.87096774193548E-3</v>
       </c>
-      <c r="AG27" s="36">
+      <c r="AG27" s="38">
         <v>39.870967741935502</v>
       </c>
       <c r="AH27" s="19" t="s">
@@ -4032,20 +4057,20 @@
       </c>
     </row>
     <row r="28" spans="1:34">
-      <c r="A28" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="B28" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="C28" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="D28" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="E28" s="48" t="s">
-        <v>177</v>
+      <c r="A28" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="D28" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>184</v>
       </c>
       <c r="F28" s="7">
         <v>1</v>
@@ -4056,17 +4081,17 @@
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="19"/>
-      <c r="K28" s="49" t="s">
-        <v>177</v>
+      <c r="K28" s="51" t="s">
+        <v>184</v>
       </c>
       <c r="L28" s="21" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="M28" s="22" t="s">
         <v>31</v>
       </c>
       <c r="N28" s="22" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="O28" s="23">
         <v>95</v>
@@ -4078,17 +4103,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R28" s="35">
+      <c r="R28" s="37">
         <v>5.91397849462366E-3</v>
       </c>
-      <c r="S28" s="36">
+      <c r="S28" s="38">
         <v>0.59139784946236595</v>
       </c>
       <c r="T28" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U28" s="37"/>
-      <c r="V28" s="38">
+      <c r="U28" s="39"/>
+      <c r="V28" s="40">
         <v>100</v>
       </c>
       <c r="W28" s="23">
@@ -4098,17 +4123,17 @@
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
-      <c r="Y28" s="35">
+      <c r="Y28" s="37">
         <v>4.6236559139784901E-3</v>
       </c>
-      <c r="Z28" s="36">
+      <c r="Z28" s="38">
         <v>5.0860215053763396</v>
       </c>
       <c r="AA28" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB28" s="37"/>
-      <c r="AC28" s="38">
+      <c r="AB28" s="39"/>
+      <c r="AC28" s="40">
         <v>300</v>
       </c>
       <c r="AD28" s="23">
@@ -4118,10 +4143,10 @@
         <f t="shared" si="2"/>
         <v>10300</v>
       </c>
-      <c r="AF28" s="35">
+      <c r="AF28" s="37">
         <v>4.1935483870967696E-3</v>
       </c>
-      <c r="AG28" s="36">
+      <c r="AG28" s="38">
         <v>43.193548387096797</v>
       </c>
       <c r="AH28" s="19" t="s">
@@ -4129,20 +4154,20 @@
       </c>
     </row>
     <row r="29" spans="1:34">
-      <c r="A29" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="B29" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="C29" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="D29" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="E29" s="48" t="s">
-        <v>183</v>
+      <c r="A29" s="50" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="D29" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" s="50" t="s">
+        <v>190</v>
       </c>
       <c r="F29" s="7">
         <v>3</v>
@@ -4153,17 +4178,17 @@
       </c>
       <c r="I29" s="18"/>
       <c r="J29" s="19"/>
-      <c r="K29" s="49" t="s">
-        <v>183</v>
+      <c r="K29" s="51" t="s">
+        <v>190</v>
       </c>
       <c r="L29" s="21" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="M29" s="22" t="s">
         <v>31</v>
       </c>
       <c r="N29" s="22" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="O29" s="23">
         <v>85</v>
@@ -4175,17 +4200,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R29" s="35">
+      <c r="R29" s="37">
         <v>2.9032258064516101E-3</v>
       </c>
-      <c r="S29" s="36">
+      <c r="S29" s="38">
         <v>0.29032258064516098</v>
       </c>
       <c r="T29" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U29" s="37"/>
-      <c r="V29" s="38">
+      <c r="U29" s="39"/>
+      <c r="V29" s="40">
         <v>100</v>
       </c>
       <c r="W29" s="23">
@@ -4195,17 +4220,17 @@
         <f t="shared" si="1"/>
         <v>3100</v>
       </c>
-      <c r="Y29" s="35">
+      <c r="Y29" s="37">
         <v>1.93548387096774E-3</v>
       </c>
-      <c r="Z29" s="36">
+      <c r="Z29" s="38">
         <v>6</v>
       </c>
       <c r="AA29" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB29" s="37"/>
-      <c r="AC29" s="38">
+      <c r="AB29" s="39"/>
+      <c r="AC29" s="40">
         <v>300</v>
       </c>
       <c r="AD29" s="23">
@@ -4215,10 +4240,10 @@
         <f t="shared" si="2"/>
         <v>30300</v>
       </c>
-      <c r="AF29" s="35">
+      <c r="AF29" s="37">
         <v>1.93548387096774E-3</v>
       </c>
-      <c r="AG29" s="36">
+      <c r="AG29" s="38">
         <v>58.645161290322598</v>
       </c>
       <c r="AH29" s="19" t="s">
@@ -4226,20 +4251,20 @@
       </c>
     </row>
     <row r="30" spans="1:34">
-      <c r="A30" s="48" t="s">
-        <v>185</v>
-      </c>
-      <c r="B30" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" s="48" t="s">
-        <v>186</v>
-      </c>
-      <c r="D30" s="48" t="s">
+      <c r="A30" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="E30" s="48" t="s">
-        <v>187</v>
+      <c r="C30" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" s="50" t="s">
+        <v>194</v>
       </c>
       <c r="F30" s="7">
         <v>1</v>
@@ -4250,17 +4275,17 @@
       </c>
       <c r="I30" s="18"/>
       <c r="J30" s="19"/>
-      <c r="K30" s="49" t="s">
-        <v>187</v>
+      <c r="K30" s="51" t="s">
+        <v>194</v>
       </c>
       <c r="L30" s="21" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="M30" s="22" t="s">
         <v>31</v>
       </c>
       <c r="N30" s="22" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="O30" s="23">
         <v>95</v>
@@ -4272,17 +4297,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R30" s="35">
+      <c r="R30" s="37">
         <v>5.4838709677419396E-3</v>
       </c>
-      <c r="S30" s="36">
+      <c r="S30" s="38">
         <v>0.54838709677419395</v>
       </c>
       <c r="T30" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U30" s="37"/>
-      <c r="V30" s="38">
+      <c r="U30" s="39"/>
+      <c r="V30" s="40">
         <v>100</v>
       </c>
       <c r="W30" s="23">
@@ -4292,17 +4317,17 @@
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
-      <c r="Y30" s="35">
+      <c r="Y30" s="37">
         <v>4.3010752688172E-3</v>
       </c>
-      <c r="Z30" s="36">
+      <c r="Z30" s="38">
         <v>4.7311827956989196</v>
       </c>
       <c r="AA30" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB30" s="37"/>
-      <c r="AC30" s="38">
+      <c r="AB30" s="39"/>
+      <c r="AC30" s="40">
         <v>300</v>
       </c>
       <c r="AD30" s="23">
@@ -4312,10 +4337,10 @@
         <f t="shared" si="2"/>
         <v>10300</v>
       </c>
-      <c r="AF30" s="35">
+      <c r="AF30" s="37">
         <v>3.87096774193548E-3</v>
       </c>
-      <c r="AG30" s="36">
+      <c r="AG30" s="38">
         <v>39.870967741935502</v>
       </c>
       <c r="AH30" s="19" t="s">
@@ -4323,20 +4348,20 @@
       </c>
     </row>
     <row r="31" spans="1:34">
-      <c r="A31" s="48" t="s">
-        <v>190</v>
-      </c>
-      <c r="B31" s="48" t="s">
-        <v>191</v>
-      </c>
-      <c r="C31" s="48" t="s">
-        <v>192</v>
-      </c>
-      <c r="D31" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="E31" s="48" t="s">
-        <v>193</v>
+      <c r="A31" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="E31" s="50" t="s">
+        <v>200</v>
       </c>
       <c r="F31" s="7">
         <v>1</v>
@@ -4347,17 +4372,17 @@
       </c>
       <c r="I31" s="18"/>
       <c r="J31" s="19"/>
-      <c r="K31" s="49" t="s">
-        <v>193</v>
+      <c r="K31" s="51" t="s">
+        <v>200</v>
       </c>
       <c r="L31" s="21" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="M31" s="22" t="s">
         <v>31</v>
       </c>
       <c r="N31" s="22" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="O31" s="23">
         <v>95</v>
@@ -4369,17 +4394,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R31" s="35">
+      <c r="R31" s="37">
         <v>2.58064516129032E-3</v>
       </c>
-      <c r="S31" s="36">
+      <c r="S31" s="38">
         <v>0.25806451612903197</v>
       </c>
       <c r="T31" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U31" s="37"/>
-      <c r="V31" s="38">
+      <c r="U31" s="39"/>
+      <c r="V31" s="40">
         <v>100</v>
       </c>
       <c r="W31" s="23">
@@ -4389,17 +4414,17 @@
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
-      <c r="Y31" s="35">
+      <c r="Y31" s="37">
         <v>1.93548387096774E-3</v>
       </c>
-      <c r="Z31" s="36">
+      <c r="Z31" s="38">
         <v>2.12903225806452</v>
       </c>
       <c r="AA31" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AB31" s="37"/>
-      <c r="AC31" s="38">
+      <c r="AB31" s="39"/>
+      <c r="AC31" s="40">
         <v>300</v>
       </c>
       <c r="AD31" s="23">
@@ -4409,10 +4434,10 @@
         <f t="shared" si="2"/>
         <v>10300</v>
       </c>
-      <c r="AF31" s="35">
+      <c r="AF31" s="37">
         <v>1.8279569892473101E-3</v>
       </c>
-      <c r="AG31" s="36">
+      <c r="AG31" s="38">
         <v>18.827956989247301</v>
       </c>
       <c r="AH31" s="19" t="s">
@@ -4420,20 +4445,20 @@
       </c>
     </row>
     <row r="32" spans="1:34">
-      <c r="A32" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="B32" s="48" t="s">
-        <v>196</v>
-      </c>
-      <c r="C32" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="D32" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="E32" s="48" t="s">
-        <v>196</v>
+      <c r="A32" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="B32" s="50" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="D32" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="E32" s="50" t="s">
+        <v>203</v>
       </c>
       <c r="F32" s="7">
         <v>12</v>
@@ -4444,17 +4469,17 @@
       </c>
       <c r="I32" s="18"/>
       <c r="J32" s="19"/>
-      <c r="K32" s="49" t="s">
-        <v>196</v>
+      <c r="K32" s="51" t="s">
+        <v>203</v>
       </c>
       <c r="L32" s="21" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="M32" s="22" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="N32" s="22" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="O32" s="23">
         <v>40</v>
@@ -4466,17 +4491,17 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="R32" s="35">
+      <c r="R32" s="37">
         <v>0.16646236559139799</v>
       </c>
-      <c r="S32" s="36">
+      <c r="S32" s="38">
         <v>16.646236559139801</v>
       </c>
       <c r="T32" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="U32" s="37"/>
-      <c r="V32" s="38">
+      <c r="U32" s="39"/>
+      <c r="V32" s="40">
         <v>100</v>
       </c>
       <c r="W32" s="23">
@@ -4486,17 +4511,17 @@
         <f t="shared" si="1"/>
         <v>12100</v>
       </c>
-      <c r="Y32" s="35">
+      <c r="Y32" s="37">
         <v>9.5989247311827994E-2</v>
       </c>
-      <c r="Z32" s="36">
+      <c r="Z32" s="38">
         <v>1161.4698924731199</v>
       </c>
       <c r="AA32" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="AB32" s="37"/>
-      <c r="AC32" s="38">
+      <c r="AB32" s="39"/>
+      <c r="AC32" s="40">
         <v>100</v>
       </c>
       <c r="AD32" s="23">
@@ -4506,10 +4531,10 @@
         <f t="shared" si="2"/>
         <v>120100</v>
       </c>
-      <c r="AF32" s="35">
+      <c r="AF32" s="37">
         <v>6.0752688172042997E-2</v>
       </c>
-      <c r="AG32" s="36">
+      <c r="AG32" s="38">
         <v>7296.3978494623698</v>
       </c>
       <c r="AH32" s="19" t="s">
@@ -4517,20 +4542,20 @@
       </c>
     </row>
     <row r="33" spans="1:34" s="2" customFormat="1" ht="15">
-      <c r="A33" s="50" t="s">
-        <v>201</v>
-      </c>
-      <c r="B33" s="50" t="s">
-        <v>202</v>
-      </c>
-      <c r="C33" s="50" t="s">
-        <v>203</v>
-      </c>
-      <c r="D33" s="50" t="s">
-        <v>204</v>
-      </c>
-      <c r="E33" s="50" t="s">
-        <v>205</v>
+      <c r="A33" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="B33" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" s="52" t="s">
+        <v>212</v>
       </c>
       <c r="F33" s="9">
         <v>1</v>
@@ -4540,86 +4565,92 @@
         <v>30</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="J33" s="25"/>
-      <c r="K33" s="51" t="s">
-        <v>205</v>
-      </c>
-      <c r="L33" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="M33" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="N33" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="K33" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="L33" s="27"/>
+      <c r="M33" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="N33" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="O33" s="28">
+      <c r="O33" s="29">
         <v>0</v>
       </c>
-      <c r="P33" s="28">
+      <c r="P33" s="29">
         <v>5</v>
       </c>
-      <c r="Q33" s="28">
+      <c r="Q33" s="29">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R33" s="40">
-        <v>0</v>
-      </c>
-      <c r="S33" s="36">
-        <v>0</v>
-      </c>
-      <c r="T33" s="25"/>
-      <c r="U33" s="41"/>
-      <c r="V33" s="39"/>
-      <c r="W33" s="28">
+      <c r="R33" s="42">
+        <v>283.87096774193498</v>
+      </c>
+      <c r="S33" s="38">
+        <v>1419.3548387096801</v>
+      </c>
+      <c r="T33" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="U33" s="43"/>
+      <c r="V33" s="41"/>
+      <c r="W33" s="29">
         <v>1000</v>
       </c>
-      <c r="X33" s="28">
+      <c r="X33" s="29">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="Y33" s="40">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA33" s="25"/>
-      <c r="AB33" s="41"/>
-      <c r="AC33" s="39"/>
-      <c r="AD33" s="28">
+      <c r="Y33" s="42">
+        <v>249.462365591398</v>
+      </c>
+      <c r="Z33" s="38">
+        <v>249462.365591398</v>
+      </c>
+      <c r="AA33" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB33" s="43"/>
+      <c r="AC33" s="41"/>
+      <c r="AD33" s="29">
         <v>10000</v>
       </c>
-      <c r="AE33" s="28">
+      <c r="AE33" s="29">
         <f t="shared" si="2"/>
         <v>10000</v>
       </c>
-      <c r="AF33" s="40">
-        <v>0</v>
-      </c>
-      <c r="AG33" s="36">
-        <v>0</v>
-      </c>
-      <c r="AH33" s="25"/>
+      <c r="AF33" s="42">
+        <v>220.43010752688201</v>
+      </c>
+      <c r="AG33" s="38">
+        <v>2204301.0752688199</v>
+      </c>
+      <c r="AH33" s="32" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="34" spans="1:34">
-      <c r="A34" s="48" t="s">
-        <v>208</v>
-      </c>
-      <c r="B34" s="48" t="s">
-        <v>209</v>
-      </c>
-      <c r="C34" s="48" t="s">
+      <c r="A34" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="B34" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="C34" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="E34" s="48" t="s">
-        <v>209</v>
+      <c r="D34" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="E34" s="50" t="s">
+        <v>218</v>
       </c>
       <c r="F34" s="7">
         <v>4</v>
@@ -4630,17 +4661,17 @@
       </c>
       <c r="I34" s="18"/>
       <c r="J34" s="19"/>
-      <c r="K34" s="49" t="s">
-        <v>209</v>
+      <c r="K34" s="51" t="s">
+        <v>218</v>
       </c>
       <c r="L34" s="21" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="M34" s="22" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="N34" s="22" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="O34" s="23">
         <v>1</v>
@@ -4652,17 +4683,17 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="R34" s="35">
+      <c r="R34" s="37">
         <v>5.0537634408602203</v>
       </c>
-      <c r="S34" s="36">
+      <c r="S34" s="38">
         <v>106.129032258065</v>
       </c>
       <c r="T34" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="U34" s="37"/>
-      <c r="V34" s="38">
+      <c r="U34" s="39"/>
+      <c r="V34" s="40">
         <v>10</v>
       </c>
       <c r="W34" s="23">
@@ -4672,17 +4703,17 @@
         <f t="shared" si="1"/>
         <v>4010</v>
       </c>
-      <c r="Y34" s="35">
+      <c r="Y34" s="37">
         <v>2.0430107526881698</v>
       </c>
-      <c r="Z34" s="36">
+      <c r="Z34" s="38">
         <v>8192.4731182795695</v>
       </c>
       <c r="AA34" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="AB34" s="37"/>
-      <c r="AC34" s="38">
+      <c r="AB34" s="39"/>
+      <c r="AC34" s="40">
         <v>15</v>
       </c>
       <c r="AD34" s="23">
@@ -4692,10 +4723,10 @@
         <f t="shared" si="2"/>
         <v>40015</v>
       </c>
-      <c r="AF34" s="35">
+      <c r="AF34" s="37">
         <v>2.02150537634409</v>
       </c>
-      <c r="AG34" s="36">
+      <c r="AG34" s="38">
         <v>80890.537634408596</v>
       </c>
       <c r="AH34" s="19" t="s">
@@ -4703,20 +4734,20 @@
       </c>
     </row>
     <row r="35" spans="1:34" s="2" customFormat="1">
-      <c r="A35" s="50" t="s">
-        <v>214</v>
-      </c>
-      <c r="B35" s="50" t="s">
-        <v>215</v>
-      </c>
-      <c r="C35" s="50" t="s">
-        <v>216</v>
-      </c>
-      <c r="D35" s="50" t="s">
-        <v>217</v>
-      </c>
-      <c r="E35" s="50" t="s">
-        <v>218</v>
+      <c r="A35" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="B35" s="52" t="s">
+        <v>224</v>
+      </c>
+      <c r="C35" s="52" t="s">
+        <v>225</v>
+      </c>
+      <c r="D35" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="E35" s="52" t="s">
+        <v>227</v>
       </c>
       <c r="F35" s="9">
         <v>1</v>
@@ -4725,95 +4756,95 @@
       <c r="H35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="30"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="51" t="s">
-        <v>218</v>
-      </c>
-      <c r="L35" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="M35" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="N35" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="O35" s="28">
+      <c r="I35" s="31"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="53" t="s">
+        <v>227</v>
+      </c>
+      <c r="L35" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="M35" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="N35" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="O35" s="29">
         <v>0</v>
       </c>
-      <c r="P35" s="28">
+      <c r="P35" s="29">
         <v>5</v>
       </c>
-      <c r="Q35" s="28">
+      <c r="Q35" s="29">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R35" s="40">
+      <c r="R35" s="42">
         <v>10.322580645161301</v>
       </c>
-      <c r="S35" s="36">
+      <c r="S35" s="38">
         <v>51.612903225806399</v>
       </c>
       <c r="T35" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="U35" s="41"/>
-      <c r="V35" s="39">
+      <c r="U35" s="43"/>
+      <c r="V35" s="41">
         <v>10</v>
       </c>
-      <c r="W35" s="28">
+      <c r="W35" s="29">
         <v>1000</v>
       </c>
-      <c r="X35" s="28">
+      <c r="X35" s="29">
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-      <c r="Y35" s="40">
+      <c r="Y35" s="42">
         <v>0.79569892473118298</v>
       </c>
-      <c r="Z35" s="36">
+      <c r="Z35" s="38">
         <v>803.65591397849505</v>
       </c>
-      <c r="AA35" s="25" t="s">
+      <c r="AA35" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="AB35" s="41"/>
-      <c r="AC35" s="39">
+      <c r="AB35" s="43"/>
+      <c r="AC35" s="41">
         <v>20</v>
       </c>
-      <c r="AD35" s="28">
+      <c r="AD35" s="29">
         <v>10000</v>
       </c>
-      <c r="AE35" s="28">
+      <c r="AE35" s="29">
         <f t="shared" si="2"/>
         <v>10020</v>
       </c>
-      <c r="AF35" s="40">
+      <c r="AF35" s="42">
         <v>0.79569892473118298</v>
       </c>
-      <c r="AG35" s="36">
+      <c r="AG35" s="38">
         <v>7972.9032258064499</v>
       </c>
-      <c r="AH35" s="25" t="s">
+      <c r="AH35" s="32" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:34" s="2" customFormat="1">
-      <c r="A36" s="50" t="s">
-        <v>222</v>
-      </c>
-      <c r="B36" s="50" t="s">
-        <v>223</v>
-      </c>
-      <c r="C36" s="50" t="s">
-        <v>216</v>
-      </c>
-      <c r="D36" s="50" t="s">
-        <v>224</v>
-      </c>
-      <c r="E36" s="50" t="s">
+      <c r="A36" s="52" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" s="52" t="s">
+        <v>232</v>
+      </c>
+      <c r="C36" s="52" t="s">
         <v>225</v>
+      </c>
+      <c r="D36" s="52" t="s">
+        <v>233</v>
+      </c>
+      <c r="E36" s="52" t="s">
+        <v>234</v>
       </c>
       <c r="F36" s="9">
         <v>1</v>
@@ -4822,95 +4853,95 @@
       <c r="H36" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="30"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="51" t="s">
-        <v>225</v>
-      </c>
-      <c r="L36" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="M36" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="N36" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="O36" s="28">
+      <c r="I36" s="31"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="53" t="s">
+        <v>234</v>
+      </c>
+      <c r="L36" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="M36" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="N36" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="O36" s="29">
         <v>0</v>
       </c>
-      <c r="P36" s="28">
+      <c r="P36" s="29">
         <v>5</v>
       </c>
-      <c r="Q36" s="28">
+      <c r="Q36" s="29">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R36" s="40">
+      <c r="R36" s="42">
         <v>4.3010752688171996</v>
       </c>
-      <c r="S36" s="36">
+      <c r="S36" s="38">
         <v>21.505376344085999</v>
       </c>
       <c r="T36" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="U36" s="41"/>
-      <c r="V36" s="39">
+      <c r="U36" s="43"/>
+      <c r="V36" s="41">
         <v>10</v>
       </c>
-      <c r="W36" s="28">
+      <c r="W36" s="29">
         <v>1000</v>
       </c>
-      <c r="X36" s="28">
+      <c r="X36" s="29">
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-      <c r="Y36" s="40">
+      <c r="Y36" s="42">
         <v>1.0752688172042999</v>
       </c>
-      <c r="Z36" s="36">
+      <c r="Z36" s="38">
         <v>1086.02150537634</v>
       </c>
-      <c r="AA36" s="25" t="s">
+      <c r="AA36" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="AB36" s="41"/>
-      <c r="AC36" s="39">
+      <c r="AB36" s="43"/>
+      <c r="AC36" s="41">
         <v>10</v>
       </c>
-      <c r="AD36" s="28">
+      <c r="AD36" s="29">
         <v>10000</v>
       </c>
-      <c r="AE36" s="28">
+      <c r="AE36" s="29">
         <f t="shared" si="2"/>
         <v>10010</v>
       </c>
-      <c r="AF36" s="40">
+      <c r="AF36" s="42">
         <v>0.91397849462365599</v>
       </c>
-      <c r="AG36" s="36">
+      <c r="AG36" s="38">
         <v>9148.9247311827894</v>
       </c>
-      <c r="AH36" s="25" t="s">
+      <c r="AH36" s="32" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:34" s="2" customFormat="1">
-      <c r="A37" s="50" t="s">
-        <v>229</v>
-      </c>
-      <c r="B37" s="50" t="s">
-        <v>230</v>
-      </c>
-      <c r="C37" s="50" t="s">
-        <v>231</v>
-      </c>
-      <c r="D37" s="50" t="s">
-        <v>232</v>
-      </c>
-      <c r="E37" s="50" t="s">
-        <v>233</v>
+      <c r="A37" s="52" t="s">
+        <v>238</v>
+      </c>
+      <c r="B37" s="52" t="s">
+        <v>239</v>
+      </c>
+      <c r="C37" s="52" t="s">
+        <v>240</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>241</v>
+      </c>
+      <c r="E37" s="52" t="s">
+        <v>242</v>
       </c>
       <c r="F37" s="9">
         <v>1</v>
@@ -4919,104 +4950,104 @@
       <c r="H37" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I37" s="30"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="51" t="s">
-        <v>233</v>
-      </c>
-      <c r="L37" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="M37" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="N37" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="O37" s="28">
+      <c r="I37" s="31"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="53" t="s">
+        <v>242</v>
+      </c>
+      <c r="L37" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="M37" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="N37" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="O37" s="29">
         <v>0</v>
       </c>
-      <c r="P37" s="28">
+      <c r="P37" s="29">
         <v>5</v>
       </c>
-      <c r="Q37" s="28">
+      <c r="Q37" s="29">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R37" s="40">
+      <c r="R37" s="42">
         <v>10.752688172042999</v>
       </c>
-      <c r="S37" s="36">
+      <c r="S37" s="38">
         <v>53.763440860214999</v>
       </c>
       <c r="T37" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="U37" s="41"/>
-      <c r="V37" s="39">
+      <c r="U37" s="43"/>
+      <c r="V37" s="41">
         <v>10</v>
       </c>
-      <c r="W37" s="28">
+      <c r="W37" s="29">
         <v>1000</v>
       </c>
-      <c r="X37" s="28">
+      <c r="X37" s="29">
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-      <c r="Y37" s="40">
+      <c r="Y37" s="42">
         <v>4.8387096774193497</v>
       </c>
-      <c r="Z37" s="36">
+      <c r="Z37" s="38">
         <v>4887.0967741935501</v>
       </c>
-      <c r="AA37" s="25" t="s">
+      <c r="AA37" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="AB37" s="41"/>
-      <c r="AC37" s="39">
+      <c r="AB37" s="43"/>
+      <c r="AC37" s="41">
         <v>10</v>
       </c>
-      <c r="AD37" s="28">
+      <c r="AD37" s="29">
         <v>10000</v>
       </c>
-      <c r="AE37" s="28">
+      <c r="AE37" s="29">
         <f t="shared" si="2"/>
         <v>10010</v>
       </c>
-      <c r="AF37" s="40">
+      <c r="AF37" s="42">
         <v>4.6236559139784896</v>
       </c>
-      <c r="AG37" s="36">
+      <c r="AG37" s="38">
         <v>46282.795698924703</v>
       </c>
-      <c r="AH37" s="25" t="s">
+      <c r="AH37" s="32" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:34" s="2" customFormat="1">
-      <c r="Q38" s="42"/>
-      <c r="R38" s="43" t="s">
+      <c r="Q38" s="44"/>
+      <c r="R38" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="S38" s="44">
+      <c r="S38" s="46">
         <f>SUM(S2:S37)</f>
-        <v>735.822150537634</v>
-      </c>
-      <c r="V38" s="45"/>
-      <c r="Y38" s="46" t="s">
+        <v>2655.6931182795702</v>
+      </c>
+      <c r="V38" s="47"/>
+      <c r="Y38" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="Z38" s="47">
+      <c r="Z38" s="49">
         <f>SUM(Z2:Z37)</f>
-        <v>73773.627741935605</v>
-      </c>
-      <c r="AC38" s="45"/>
-      <c r="AF38" s="46" t="s">
+        <v>367776.13452688197</v>
+      </c>
+      <c r="AC38" s="47"/>
+      <c r="AF38" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="AG38" s="47">
+      <c r="AG38" s="49">
         <f>SUM(AG2:AG37)</f>
-        <v>657224.45763440803</v>
+        <v>3300043.0597849502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>